<commit_message>
aug 31 fixed few issue office evening
</commit_message>
<xml_diff>
--- a/LOGS/712a6d97-dc33-4cb8-b5ca-e56dae5dd169/main_page_service_output/main_pages.xlsx
+++ b/LOGS/712a6d97-dc33-4cb8-b5ca-e56dae5dd169/main_page_service_output/main_pages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="104">
   <si>
     <t>Particulars</t>
   </si>
@@ -30,6 +30,99 @@
     <t>statement_sub_section</t>
   </si>
   <si>
+    <t>ASSETS</t>
+  </si>
+  <si>
+    <t>Current assets</t>
+  </si>
+  <si>
+    <t>Cash and cash equivalents</t>
+  </si>
+  <si>
+    <t>Trade and other receivables</t>
+  </si>
+  <si>
+    <t>Contract assets</t>
+  </si>
+  <si>
+    <t>Inventories</t>
+  </si>
+  <si>
+    <t>Other assets</t>
+  </si>
+  <si>
+    <t>Total current assets</t>
+  </si>
+  <si>
+    <t>Non-current assets</t>
+  </si>
+  <si>
+    <t>Property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Intangible assets</t>
+  </si>
+  <si>
+    <t>Other Non-Current Assets</t>
+  </si>
+  <si>
+    <t>Total non-current assets</t>
+  </si>
+  <si>
+    <t>Total assets</t>
+  </si>
+  <si>
+    <t>LIABILITIES</t>
+  </si>
+  <si>
+    <t>Current liabilities</t>
+  </si>
+  <si>
+    <t>Trade and other payables</t>
+  </si>
+  <si>
+    <t>Contract liabilities</t>
+  </si>
+  <si>
+    <t>Provisions</t>
+  </si>
+  <si>
+    <t>Financialliabilities</t>
+  </si>
+  <si>
+    <t>Lease liabilities</t>
+  </si>
+  <si>
+    <t>Current tax liabilities</t>
+  </si>
+  <si>
+    <t>Deferred vendor payments current</t>
+  </si>
+  <si>
+    <t>Total current liabilities</t>
+  </si>
+  <si>
+    <t>Non-current liabilities</t>
+  </si>
+  <si>
+    <t>Financial liabilities</t>
+  </si>
+  <si>
+    <t>Deferred vendor payments - non-current</t>
+  </si>
+  <si>
+    <t>Deferred tax liabilities</t>
+  </si>
+  <si>
+    <t>Total non-current liabilities</t>
+  </si>
+  <si>
+    <t>Total liabilities</t>
+  </si>
+  <si>
+    <t>Net assets</t>
+  </si>
+  <si>
     <t>EQUITY</t>
   </si>
   <si>
@@ -51,9 +144,18 @@
     <t>3.18</t>
   </si>
   <si>
+    <t>assets</t>
+  </si>
+  <si>
     <t>equity_liabilities</t>
   </si>
   <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>noncurrent</t>
+  </si>
+  <si>
     <t>equity</t>
   </si>
   <si>
@@ -216,13 +318,13 @@
     <t>Cash and cash equivalents at end of reporting period</t>
   </si>
   <si>
+    <t>operating_activities</t>
+  </si>
+  <si>
+    <t>investing_activities</t>
+  </si>
+  <si>
     <t>financing_activities</t>
-  </si>
-  <si>
-    <t>operating_activities</t>
-  </si>
-  <si>
-    <t>investing_activities</t>
   </si>
   <si>
     <t>net_working_capital</t>
@@ -583,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -620,84 +722,739 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3">
-        <v>241295</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>241295</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="C4">
-        <v>2038</v>
+        <v>12892</v>
       </c>
       <c r="D4">
-        <v>2171</v>
+        <v>30545</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5">
+        <v>3.4</v>
+      </c>
       <c r="C5">
-        <v>93128</v>
+        <v>51750</v>
       </c>
       <c r="D5">
-        <v>71901</v>
+        <v>74169</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6">
+        <v>3.5</v>
+      </c>
       <c r="C6">
+        <v>57671</v>
+      </c>
+      <c r="D6">
+        <v>26543</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1518</v>
+      </c>
+      <c r="D7">
+        <v>1306</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>3.6</v>
+      </c>
+      <c r="C8">
+        <v>5898</v>
+      </c>
+      <c r="D8">
+        <v>10665</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>129729</v>
+      </c>
+      <c r="D9">
+        <v>158774</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>3.4</v>
+      </c>
+      <c r="C11">
+        <v>10034</v>
+      </c>
+      <c r="D11">
+        <v>262</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>3.5</v>
+      </c>
+      <c r="C12">
+        <v>11792</v>
+      </c>
+      <c r="D12">
+        <v>13240</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3.7</v>
+      </c>
+      <c r="C13">
+        <v>22185</v>
+      </c>
+      <c r="D13">
+        <v>28044</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>3.8</v>
+      </c>
+      <c r="C14">
+        <v>412452</v>
+      </c>
+      <c r="D14">
+        <v>400852</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>3.6</v>
+      </c>
+      <c r="C15">
+        <v>1819</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>458282</v>
+      </c>
+      <c r="D16">
+        <v>442398</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>588011</v>
+      </c>
+      <c r="D17">
+        <v>601172</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>3.1</v>
+      </c>
+      <c r="C20">
+        <v>25069</v>
+      </c>
+      <c r="D20">
+        <v>32512</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>3.13</v>
+      </c>
+      <c r="C21">
+        <v>9451</v>
+      </c>
+      <c r="D21">
+        <v>14402</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>3.12</v>
+      </c>
+      <c r="C22">
+        <v>21962</v>
+      </c>
+      <c r="D22">
+        <v>28382</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>3.11</v>
+      </c>
+      <c r="C23">
+        <v>15000</v>
+      </c>
+      <c r="D23">
+        <v>17000</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>3.14</v>
+      </c>
+      <c r="C24">
+        <v>5055</v>
+      </c>
+      <c r="D24">
+        <v>6931</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>3.9</v>
+      </c>
+      <c r="C25">
+        <v>144</v>
+      </c>
+      <c r="D25">
+        <v>146</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>3.15</v>
+      </c>
+      <c r="C26">
+        <v>33706</v>
+      </c>
+      <c r="D26">
+        <v>63082</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>110387</v>
+      </c>
+      <c r="D27">
+        <v>162455</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>3.12</v>
+      </c>
+      <c r="C29">
+        <v>1501</v>
+      </c>
+      <c r="D29">
+        <v>1314</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>3.11</v>
+      </c>
+      <c r="C30">
+        <v>109000</v>
+      </c>
+      <c r="D30">
+        <v>70000</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>3.14</v>
+      </c>
+      <c r="C31">
+        <v>8287</v>
+      </c>
+      <c r="D31">
+        <v>11338</v>
+      </c>
+      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>3.15</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>24304</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>3.9</v>
+      </c>
+      <c r="C33">
+        <v>22376</v>
+      </c>
+      <c r="D33">
+        <v>16394</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>141164</v>
+      </c>
+      <c r="D34">
+        <v>123350</v>
+      </c>
+      <c r="E34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>251551</v>
+      </c>
+      <c r="D35">
+        <v>285805</v>
+      </c>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36">
         <v>336461</v>
       </c>
-      <c r="D6">
+      <c r="D36">
         <v>315367</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38">
+        <v>241295</v>
+      </c>
+      <c r="D38">
+        <v>241295</v>
+      </c>
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39">
+        <v>2038</v>
+      </c>
+      <c r="D39">
+        <v>2171</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>93128</v>
+      </c>
+      <c r="D40">
+        <v>71901</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <v>336461</v>
+      </c>
+      <c r="D41">
+        <v>315367</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -729,10 +1486,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C2">
         <v>394534</v>
@@ -743,7 +1500,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>1272</v>
@@ -754,7 +1511,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>395806</v>
@@ -765,7 +1522,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>12268</v>
@@ -776,7 +1533,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -787,7 +1544,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>1492</v>
@@ -798,7 +1555,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>-50957</v>
@@ -809,7 +1566,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <v>-285150</v>
@@ -820,7 +1577,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>-20774</v>
@@ -831,7 +1588,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C11">
         <v>-8025</v>
@@ -842,7 +1599,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C12">
         <v>-15300</v>
@@ -853,7 +1610,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>-237</v>
@@ -864,7 +1621,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>-378951</v>
@@ -875,7 +1632,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C15">
         <v>29123</v>
@@ -886,10 +1643,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C16">
         <v>-7896</v>
@@ -900,7 +1657,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C17">
         <v>21227</v>
@@ -911,7 +1668,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>-133</v>
@@ -922,7 +1679,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C19">
         <v>21094</v>
@@ -963,7 +1720,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -972,12 +1729,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>29123</v>
@@ -986,12 +1743,12 @@
         <v>51250</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1000,12 +1757,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1014,12 +1771,12 @@
         <v>157</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B6">
         <v>20775</v>
@@ -1028,12 +1785,12 @@
         <v>26795</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B7">
         <v>8026</v>
@@ -1042,12 +1799,12 @@
         <v>6764</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B8">
         <v>-255</v>
@@ -1056,12 +1813,12 @@
         <v>-21</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>-1492</v>
@@ -1070,12 +1827,12 @@
         <v>-584</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>-11116</v>
@@ -1084,12 +1841,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1098,12 +1855,15 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>100</v>
+      </c>
+      <c r="E11" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="B12">
         <v>8401</v>
@@ -1112,15 +1872,15 @@
         <v>-32688</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1129,15 +1889,15 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B14">
         <v>-211</v>
@@ -1146,15 +1906,15 @@
         <v>-650</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>2946</v>
@@ -1163,15 +1923,15 @@
         <v>678</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <v>-17761</v>
@@ -1180,15 +1940,15 @@
         <v>20843</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1197,15 +1957,15 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B18">
         <v>-145</v>
@@ -1214,15 +1974,15 @@
         <v>-2722</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B19">
         <v>255</v>
@@ -1231,15 +1991,15 @@
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="B20">
         <v>-3575</v>
@@ -1248,15 +2008,15 @@
         <v>-1707</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B21">
         <v>-11804</v>
@@ -1265,12 +2025,12 @@
         <v>-16742</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B22">
         <v>23167</v>
@@ -1279,12 +2039,12 @@
         <v>51394</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1293,12 +2053,12 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B24">
         <v>-2868</v>
@@ -1307,12 +2067,12 @@
         <v>-3073</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B25">
         <v>-5498</v>
@@ -1321,12 +2081,12 @@
         <v>-8568</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>-63700</v>
@@ -1335,12 +2095,12 @@
         <v>-93477</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B27">
         <v>-72066</v>
@@ -1349,12 +2109,12 @@
         <v>-105118</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1363,12 +2123,12 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="B29">
         <v>83000</v>
@@ -1377,12 +2137,12 @@
         <v>82000</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B30">
         <v>-46000</v>
@@ -1391,12 +2151,12 @@
         <v>-12000</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="B31">
         <v>-5754</v>
@@ -1405,12 +2165,12 @@
         <v>-8657</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1419,12 +2179,12 @@
         <v>10000</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B33">
         <v>31246</v>
@@ -1433,12 +2193,12 @@
         <v>71343</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1447,12 +2207,12 @@
         <v>-421</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="B35">
         <v>-17653</v>
@@ -1461,12 +2221,12 @@
         <v>17198</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="B36">
         <v>30545</v>
@@ -1475,12 +2235,12 @@
         <v>13347</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="B37">
         <v>12892</v>
@@ -1489,7 +2249,7 @@
         <v>30545</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>